<commit_message>
contact for t session
</commit_message>
<xml_diff>
--- a/task/contacts_training_session.xlsx
+++ b/task/contacts_training_session.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ad0791/Desktop/Hanwash.mwater.dev/task/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D82578-16E5-8340-81D3-DFCAAC696F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DF55F0-7A60-964D-B3C1-907CED3097E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="1040" windowWidth="24640" windowHeight="14360" activeTab="4" xr2:uid="{EB43E17C-C815-E048-94EE-CA24FF1D354D}"/>
   </bookViews>
@@ -159,12 +159,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -173,14 +188,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -550,7 +566,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,90 +576,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
All the piece of the UI are done for now
</commit_message>
<xml_diff>
--- a/task/contacts_training_session.xlsx
+++ b/task/contacts_training_session.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ad0791/Desktop/Hanwash.mwater.dev/task/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A39819-A84D-594F-AC5F-000C25C205A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F26A463-9FCD-674E-B586-0A13AA67428E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="4" xr2:uid="{EB43E17C-C815-E048-94EE-CA24FF1D354D}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>name</t>
   </si>
@@ -148,6 +148,30 @@
   </si>
   <si>
     <t>project team?</t>
+  </si>
+  <si>
+    <t>Haiti Liaison</t>
+  </si>
+  <si>
+    <t>Steering Committee</t>
+  </si>
+  <si>
+    <t>M&amp;E Committee and Hanwash Staff</t>
+  </si>
+  <si>
+    <t>Project Team cavaillon</t>
+  </si>
+  <si>
+    <t>Project Team ferrier</t>
+  </si>
+  <si>
+    <t>Project Team leogane</t>
+  </si>
+  <si>
+    <t>Project Team terre neuve</t>
+  </si>
+  <si>
+    <t>Project Team pignon</t>
   </si>
 </sst>
 </file>
@@ -257,7 +281,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -280,18 +304,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -656,10 +679,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408CC4F2-00A9-4341-AF06-6E6E1714976E}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,10 +781,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -769,10 +792,10 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -783,7 +806,7 @@
       <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -794,7 +817,7 @@
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -805,7 +828,7 @@
       <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -813,11 +836,71 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10" t="s">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="9"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="12">
+        <v>45579</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="12">
+        <v>45586</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="11"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="12">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="11"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="11"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="11"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="11"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
email for training session
</commit_message>
<xml_diff>
--- a/task/contacts_training_session.xlsx
+++ b/task/contacts_training_session.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ad0791/Desktop/Hanwash.mwater.dev/task/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A2EB25-2B06-DA4C-B686-E897AC8802A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9864A624-C7F6-8442-B234-DF81540E14B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="4" xr2:uid="{EB43E17C-C815-E048-94EE-CA24FF1D354D}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>name</t>
   </si>
@@ -172,6 +172,15 @@
   </si>
   <si>
     <t>Project Team pignon</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>contacted</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -281,7 +290,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -316,6 +325,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -680,10 +692,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408CC4F2-00A9-4341-AF06-6E6E1714976E}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -843,59 +855,90 @@
       </c>
       <c r="C14" s="8"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="12">
-        <v>45579</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="12"/>
+      <c r="C18" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="15">
+        <v>45589</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="12"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="12">
+        <v>45600</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="15">
+        <v>45587</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="13"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="15">
+        <v>45589</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="12">
-        <v>45576</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="12"/>
+      <c r="C21" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="15">
+        <v>45589</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="11"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="11"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="11"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B25" s="11"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
move like a man
</commit_message>
<xml_diff>
--- a/task/contacts_training_session.xlsx
+++ b/task/contacts_training_session.xlsx
@@ -8,18 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ad0791/Desktop/Hanwash.mwater.dev/task/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB92829-9606-5B42-AA1B-EBE716B5E382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B0DB35-7204-E24F-8825-21A64ED4672A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="4" xr2:uid="{EB43E17C-C815-E048-94EE-CA24FF1D354D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{EB43E17C-C815-E048-94EE-CA24FF1D354D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Haiti_Liason_leaders" sheetId="1" r:id="rId1"/>
-    <sheet name="m&amp;e_committee" sheetId="2" r:id="rId2"/>
-    <sheet name="steering_committee_leaders" sheetId="3" r:id="rId3"/>
-    <sheet name="D 7020 Leaders" sheetId="4" r:id="rId4"/>
-    <sheet name="training_sessions" sheetId="5" r:id="rId5"/>
+    <sheet name="training_sessions" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
   <si>
     <t>name</t>
   </si>
@@ -187,6 +184,60 @@
   </si>
   <si>
     <t>contact_date</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>email or phones</t>
+  </si>
+  <si>
+    <t>Jean Marie Naissant</t>
+  </si>
+  <si>
+    <t>Mayors</t>
+  </si>
+  <si>
+    <t>Maire de Cavaillon</t>
+  </si>
+  <si>
+    <t>Ernson Henry</t>
+  </si>
+  <si>
+    <t>Maire de Leogane</t>
+  </si>
+  <si>
+    <t>+509 38 06 4195</t>
+  </si>
+  <si>
+    <t>Yvette Guerrier</t>
+  </si>
+  <si>
+    <t>Maire Ferrier</t>
+  </si>
+  <si>
+    <t>+509 43 30 8841 41971354/ 37665303</t>
+  </si>
+  <si>
+    <t>Henry Claude Crepin</t>
+  </si>
+  <si>
+    <t>Maire Pignon</t>
+  </si>
+  <si>
+    <t>+509 40027666</t>
+  </si>
+  <si>
+    <t>Raymond Joanel</t>
+  </si>
+  <si>
+    <t>Maire Terre-Neuve</t>
+  </si>
+  <si>
+    <t>+509 32157300</t>
+  </si>
+  <si>
+    <t>+50932918761/+50948620579</t>
   </si>
 </sst>
 </file>
@@ -296,7 +347,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -334,6 +385,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -649,59 +704,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9499075C-D33E-5345-862B-374667119FDF}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714C799F-C65E-6E40-A139-3E18AB4FA2A3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6653352A-8AF2-DF48-8CBF-540B1AA959E0}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85D3557-7598-C346-B867-5863EA857D3D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408CC4F2-00A9-4341-AF06-6E6E1714976E}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -973,4 +980,90 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5A553B-73E7-E54E-9F4F-BF5D1FBA8B51}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="77" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="50.83203125" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="38.33203125" style="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
work with the pres
</commit_message>
<xml_diff>
--- a/task/contacts_training_session.xlsx
+++ b/task/contacts_training_session.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ad0791/Desktop/Hanwash.mwater.dev/task/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDEBA45-9B6B-514F-A3D0-6B3ED8E74C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507E5EFA-087B-C242-9DCC-586F5F69A435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{EB43E17C-C815-E048-94EE-CA24FF1D354D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
   <si>
     <t>name</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>raymondjoanel4862@gmail.com</t>
+  </si>
+  <si>
+    <t>guerrierivette@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1019,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="77" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1081,12 +1084,14 @@
       <c r="B4" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="23" t="s">
+        <v>70</v>
+      </c>
       <c r="D4" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>68</v>
+      <c r="E4" s="22" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1096,7 +1101,7 @@
       <c r="B5" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="20" t="s">
         <v>62</v>
       </c>
@@ -1124,6 +1129,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1" xr:uid="{B204C191-0E4F-DA44-BB18-BBB56D90171E}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{DBDDDC87-CEE6-A54C-8221-7F454C90CB64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>